<commit_message>
Update CORS settings and ALLOWED_HOSTS for better security and compatibility
</commit_message>
<xml_diff>
--- a/render-site.-info.xlsx
+++ b/render-site.-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\tamrin_webgis\version5-ant\webgis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04739C5-786E-46F4-A884-CCFDE1CB431C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0482F4C-FC0A-4C51-B0D7-136C3AB552BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{07390BCF-D395-4A43-8799-8EDA575BF3CB}"/>
+    <workbookView xWindow="1296" yWindow="540" windowWidth="15144" windowHeight="12348" xr2:uid="{07390BCF-D395-4A43-8799-8EDA575BF3CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -439,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211E74BB-9C9D-4464-8747-FE6D3DBD96DD}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,72 +456,72 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5432</v>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>